<commit_message>
Cutting probabilities as command line arguments
Added mutation cutting probabilities as command line arguments
Params Constructor is now simpler
</commit_message>
<xml_diff>
--- a/Results/Excel Sheets/First Comparison.xlsx
+++ b/Results/Excel Sheets/First Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diogo\OneDrive\Documentos\IST\Master Thesis\MADCoM\Results\Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE36A8A0-DC01-4D37-BD4E-035C7863B952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C115F37A-58D5-4168-9F7D-16CC41A92B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{03D7EE80-680F-421B-99E1-BEBDEF059FA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{03D7EE80-680F-421B-99E1-BEBDEF059FA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="28">
   <si>
     <t>Instance</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>NºTasks</t>
+  </si>
+  <si>
+    <t>madcom -mutprob 0</t>
+  </si>
+  <si>
+    <t>madcom -mutprob 0.5</t>
   </si>
 </sst>
 </file>
@@ -458,11 +464,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -473,14 +483,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -491,7 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,7 +509,812 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="160">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1131,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EEBC759-3513-4B3C-9D29-C75598F3A089}">
   <dimension ref="A2:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -1143,64 +1954,64 @@
   <sheetData>
     <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="45" t="s">
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="45" t="s">
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="45" t="s">
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
+      <c r="R3" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="46"/>
-      <c r="T3" s="46"/>
-      <c r="U3" s="47"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="49"/>
     </row>
     <row r="4" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="43" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="43" t="s">
+      <c r="I4" s="51"/>
+      <c r="J4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="43" t="s">
+      <c r="K4" s="51"/>
+      <c r="L4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="44"/>
-      <c r="N4" s="43" t="s">
+      <c r="M4" s="51"/>
+      <c r="N4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="43" t="s">
+      <c r="O4" s="51"/>
+      <c r="P4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="43" t="s">
+      <c r="Q4" s="51"/>
+      <c r="R4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="44"/>
-      <c r="T4" s="43" t="s">
+      <c r="S4" s="51"/>
+      <c r="T4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="44"/>
+      <c r="U4" s="51"/>
     </row>
     <row r="5" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="str">
@@ -1265,7 +2076,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1339,7 +2150,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="19" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +2222,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="19" t="s">
         <v>14</v>
       </c>
@@ -1483,7 +2294,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="49"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="19" t="s">
         <v>8</v>
       </c>
@@ -1555,7 +2366,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="30" t="s">
         <v>15</v>
       </c>
@@ -1674,51 +2485,51 @@
     </row>
     <row r="13" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="45" t="s">
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="46"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="47"/>
-      <c r="N13" s="45" t="s">
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="47"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="49"/>
     </row>
     <row r="14" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="43" t="s">
+      <c r="G14" s="51"/>
+      <c r="H14" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="43" t="s">
+      <c r="I14" s="51"/>
+      <c r="J14" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="44"/>
-      <c r="L14" s="43" t="s">
+      <c r="K14" s="51"/>
+      <c r="L14" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="44"/>
-      <c r="N14" s="43" t="s">
+      <c r="M14" s="51"/>
+      <c r="N14" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="44"/>
-      <c r="P14" s="43" t="s">
+      <c r="O14" s="51"/>
+      <c r="P14" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="Q14" s="44"/>
+      <c r="Q14" s="51"/>
     </row>
     <row r="15" spans="1:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="26"/>
@@ -1773,7 +2584,7 @@
     </row>
     <row r="16" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -1836,7 +2647,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
-      <c r="B17" s="49"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="19" t="s">
         <v>13</v>
       </c>
@@ -1896,7 +2707,7 @@
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="49"/>
+      <c r="B18" s="45"/>
       <c r="C18" s="19" t="s">
         <v>14</v>
       </c>
@@ -1956,7 +2767,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="49"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="19" t="s">
         <v>8</v>
       </c>
@@ -2016,7 +2827,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="50"/>
+      <c r="B20" s="46"/>
       <c r="C20" s="30" t="s">
         <v>15</v>
       </c>
@@ -2078,6 +2889,13 @@
     <row r="21" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="R3:U3"/>
     <mergeCell ref="R4:S4"/>
@@ -2094,58 +2912,51 @@
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <conditionalFormatting sqref="G6 K6 O6">
-    <cfRule type="top10" dxfId="44" priority="14" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="159" priority="14" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7 K7 O7">
-    <cfRule type="top10" dxfId="43" priority="15" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="158" priority="15" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8 K8 O8">
-    <cfRule type="top10" dxfId="42" priority="13" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="157" priority="13" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9 K9 O9">
-    <cfRule type="top10" dxfId="41" priority="12" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="156" priority="12" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 K10 O10">
-    <cfRule type="top10" dxfId="40" priority="11" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="155" priority="11" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16 K16 O16">
-    <cfRule type="top10" dxfId="39" priority="10" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="154" priority="10" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17 K17 O17">
-    <cfRule type="top10" dxfId="38" priority="9" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="153" priority="9" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18 K18 O18">
-    <cfRule type="top10" dxfId="37" priority="8" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="152" priority="8" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19 K19 O19">
-    <cfRule type="top10" dxfId="36" priority="7" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="151" priority="7" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20 K20 O20">
-    <cfRule type="top10" dxfId="35" priority="6" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="150" priority="6" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16 M16 Q16">
-    <cfRule type="top10" dxfId="34" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="149" priority="5" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17 M17 Q17">
-    <cfRule type="top10" dxfId="33" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="148" priority="4" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18 M18 Q18">
-    <cfRule type="top10" dxfId="32" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="147" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19 M19 Q19">
-    <cfRule type="top10" dxfId="31" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="146" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20 M20 Q20">
-    <cfRule type="top10" dxfId="30" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="145" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2170,18 +2981,18 @@
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="24"/>
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="44"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="7" t="s">
@@ -2223,21 +3034,21 @@
       <c r="O3" s="4">
         <v>10</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="43" t="s">
+      <c r="Q3" s="51"/>
+      <c r="R3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="44"/>
+      <c r="S3" s="51"/>
       <c r="T3" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="11" t="str">
@@ -2305,7 +3116,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="49"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="11" t="str">
         <f>Comparison!C7</f>
         <v>F1_g-6</v>
@@ -2371,7 +3182,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="49"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="11" t="str">
         <f>Comparison!C8</f>
         <v>Beijing-3</v>
@@ -2437,7 +3248,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="49"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="11" t="str">
         <f>Comparison!C9</f>
         <v>Hefei-10</v>
@@ -2503,7 +3314,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="49"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="11" t="str">
         <f>Comparison!C10</f>
         <v>Beijing-5</v>
@@ -2569,7 +3380,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="49"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="11"/>
       <c r="D9" s="21"/>
       <c r="E9" s="17"/>
@@ -2591,7 +3402,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="49"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="11"/>
       <c r="D10" s="21"/>
       <c r="E10" s="17"/>
@@ -2612,7 +3423,7 @@
       <c r="T10" s="21"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="49"/>
+      <c r="B11" s="45"/>
       <c r="E11" s="5"/>
       <c r="P11" s="5"/>
       <c r="Q11" s="6"/>
@@ -2621,7 +3432,7 @@
       <c r="T11" s="5"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="49"/>
+      <c r="B12" s="45"/>
       <c r="E12" s="5"/>
       <c r="P12" s="5"/>
       <c r="Q12" s="6"/>
@@ -2630,7 +3441,7 @@
       <c r="T12" s="5"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="45"/>
       <c r="E13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="6"/>
@@ -2667,18 +3478,18 @@
     </row>
     <row r="16" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="26"/>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="44"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11"/>
@@ -2721,20 +3532,20 @@
       <c r="O17" s="2">
         <v>10</v>
       </c>
-      <c r="P17" s="43" t="s">
+      <c r="P17" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="43" t="s">
+      <c r="Q17" s="51"/>
+      <c r="R17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S17" s="44"/>
+      <c r="S17" s="51"/>
       <c r="T17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="11" t="str">
@@ -2801,7 +3612,7 @@
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="49"/>
+      <c r="B19" s="45"/>
       <c r="C19" s="11" t="str">
         <f>Comparison!C7</f>
         <v>F1_g-6</v>
@@ -2866,7 +3677,7 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="11" t="str">
         <f>Comparison!C8</f>
         <v>Beijing-3</v>
@@ -2931,7 +3742,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="49"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="11" t="str">
         <f>Comparison!C9</f>
         <v>Hefei-10</v>
@@ -2996,7 +3807,7 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="49"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="11" t="str">
         <f>Comparison!C10</f>
         <v>Beijing-5</v>
@@ -3061,7 +3872,7 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="49"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="11"/>
       <c r="D23" s="21"/>
       <c r="E23" s="17"/>
@@ -3082,7 +3893,7 @@
       <c r="T23" s="21"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="49"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="11"/>
       <c r="D24" s="21"/>
       <c r="E24" s="17"/>
@@ -3103,7 +3914,7 @@
       <c r="T24" s="21"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="49"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="11"/>
       <c r="D25" s="21"/>
       <c r="E25" s="17"/>
@@ -3124,7 +3935,7 @@
       <c r="T25" s="21"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="49"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="11"/>
       <c r="D26" s="21"/>
       <c r="E26" s="17"/>
@@ -3145,7 +3956,7 @@
       <c r="T26" s="21"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="49"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="11"/>
       <c r="D27" s="21"/>
       <c r="E27" s="17"/>
@@ -3217,18 +4028,18 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="44"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
@@ -3271,21 +4082,21 @@
       <c r="O3" s="2">
         <v>10</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="43" t="s">
+      <c r="Q3" s="51"/>
+      <c r="R3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="44"/>
+      <c r="S3" s="51"/>
       <c r="T3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="11" t="str">
@@ -3353,7 +4164,7 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
-      <c r="B5" s="49"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="11" t="str">
         <f>Comparison!C7</f>
         <v>F1_g-6</v>
@@ -3419,7 +4230,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
-      <c r="B6" s="49"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="11" t="str">
         <f>Comparison!C8</f>
         <v>Beijing-3</v>
@@ -3485,7 +4296,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
-      <c r="B7" s="49"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="11" t="str">
         <f>Comparison!C9</f>
         <v>Hefei-10</v>
@@ -3551,7 +4362,7 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
-      <c r="B8" s="49"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="11" t="str">
         <f>Comparison!C10</f>
         <v>Beijing-5</v>
@@ -3617,7 +4428,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
-      <c r="B9" s="49"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="11"/>
       <c r="D9" s="21"/>
       <c r="E9" s="17"/>
@@ -3639,7 +4450,7 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
-      <c r="B10" s="49"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="11"/>
       <c r="D10" s="21"/>
       <c r="E10" s="17"/>
@@ -3661,7 +4472,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="49"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11"/>
       <c r="D11" s="21"/>
       <c r="E11" s="17"/>
@@ -3673,7 +4484,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
-      <c r="B12" s="49"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="11"/>
       <c r="D12" s="21"/>
       <c r="E12" s="17"/>
@@ -3685,7 +4496,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
-      <c r="B13" s="49"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="11"/>
       <c r="D13" s="21"/>
       <c r="E13" s="17"/>
@@ -3697,7 +4508,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
-      <c r="B14" s="49"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="11"/>
       <c r="D14" s="21"/>
       <c r="E14" s="17"/>
@@ -3720,18 +4531,18 @@
     <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="44"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="51"/>
     </row>
     <row r="18" spans="2:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11"/>
@@ -3774,20 +4585,20 @@
       <c r="O18" s="2">
         <v>10</v>
       </c>
-      <c r="P18" s="43" t="s">
+      <c r="P18" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="43" t="s">
+      <c r="Q18" s="51"/>
+      <c r="R18" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S18" s="44"/>
+      <c r="S18" s="51"/>
       <c r="T18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="11" t="str">
@@ -3854,7 +4665,7 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="11" t="str">
         <f>Comparison!C7</f>
         <v>F1_g-6</v>
@@ -3919,7 +4730,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="49"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="11" t="str">
         <f>Comparison!C8</f>
         <v>Beijing-3</v>
@@ -3984,7 +4795,7 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="49"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="11" t="str">
         <f>Comparison!C9</f>
         <v>Hefei-10</v>
@@ -4049,7 +4860,7 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="49"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="11" t="str">
         <f>Comparison!C10</f>
         <v>Beijing-5</v>
@@ -4114,7 +4925,7 @@
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="49"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="11"/>
       <c r="D24" s="21"/>
       <c r="E24" s="17"/>
@@ -4135,7 +4946,7 @@
       <c r="T24" s="21"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="49"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="11"/>
       <c r="D25" s="21"/>
       <c r="E25" s="17"/>
@@ -4156,7 +4967,7 @@
       <c r="T25" s="21"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="49"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="11"/>
       <c r="D26" s="21"/>
       <c r="E26" s="17"/>
@@ -4177,7 +4988,7 @@
       <c r="T26" s="21"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="49"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="11"/>
       <c r="D27" s="21"/>
       <c r="E27" s="17"/>
@@ -4198,7 +5009,7 @@
       <c r="T27" s="21"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="49"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="11"/>
       <c r="D28" s="21"/>
       <c r="E28" s="17"/>
@@ -4257,7 +5068,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A981BF-362D-4F38-A22D-B817C4C20373}">
   <dimension ref="B1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -4265,18 +5076,18 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="43" t="s">
+      <c r="F2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="44"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
@@ -4319,20 +5130,20 @@
       <c r="O3" s="2">
         <v>10</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="43" t="s">
+      <c r="Q3" s="51"/>
+      <c r="R3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="44"/>
+      <c r="S3" s="51"/>
       <c r="T3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="11" t="str">
@@ -4399,7 +5210,7 @@
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
+      <c r="B5" s="45"/>
       <c r="C5" s="11" t="str">
         <f>Comparison!C7</f>
         <v>F1_g-6</v>
@@ -4464,7 +5275,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="49"/>
+      <c r="B6" s="45"/>
       <c r="C6" s="11" t="str">
         <f>Comparison!C8</f>
         <v>Beijing-3</v>
@@ -4529,7 +5340,7 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="11" t="str">
         <f>Comparison!C9</f>
         <v>Hefei-10</v>
@@ -4594,7 +5405,7 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="11" t="str">
         <f>Comparison!C10</f>
         <v>Beijing-5</v>
@@ -4659,7 +5470,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="49"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="11"/>
       <c r="D9" s="21"/>
       <c r="E9" s="17"/>
@@ -4680,7 +5491,7 @@
       <c r="T9" s="21"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="49"/>
+      <c r="B10" s="45"/>
       <c r="C10" s="11"/>
       <c r="D10" s="21"/>
       <c r="E10" s="17"/>
@@ -4691,7 +5502,7 @@
       <c r="T10" s="21"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B11" s="49"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11"/>
       <c r="D11" s="21"/>
       <c r="E11" s="17"/>
@@ -4702,7 +5513,7 @@
       <c r="T11" s="21"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B12" s="49"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="11"/>
       <c r="D12" s="21"/>
       <c r="E12" s="17"/>
@@ -4713,7 +5524,7 @@
       <c r="T12" s="21"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="11"/>
       <c r="D13" s="21"/>
       <c r="E13" s="17"/>
@@ -4734,7 +5545,7 @@
       <c r="T13" s="21"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="49"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="11"/>
       <c r="D14" s="21"/>
       <c r="E14" s="17"/>
@@ -4757,18 +5568,18 @@
     <row r="16" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="26"/>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="44"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="51"/>
     </row>
     <row r="18" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11"/>
@@ -4811,20 +5622,20 @@
       <c r="O18" s="2">
         <v>10</v>
       </c>
-      <c r="P18" s="43" t="s">
+      <c r="P18" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="43" t="s">
+      <c r="Q18" s="51"/>
+      <c r="R18" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S18" s="44"/>
+      <c r="S18" s="51"/>
       <c r="T18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="44" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="11" t="str">
@@ -4891,7 +5702,7 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="49"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="11" t="str">
         <f>Comparison!C7</f>
         <v>F1_g-6</v>
@@ -4956,7 +5767,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="49"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="11" t="str">
         <f>Comparison!C8</f>
         <v>Beijing-3</v>
@@ -5021,7 +5832,7 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="49"/>
+      <c r="B22" s="45"/>
       <c r="C22" s="11" t="str">
         <f>Comparison!C9</f>
         <v>Hefei-10</v>
@@ -5086,7 +5897,7 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="49"/>
+      <c r="B23" s="45"/>
       <c r="C23" s="11" t="str">
         <f>Comparison!C10</f>
         <v>Beijing-5</v>
@@ -5151,7 +5962,7 @@
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="49"/>
+      <c r="B24" s="45"/>
       <c r="C24" s="11"/>
       <c r="D24" s="21"/>
       <c r="E24" s="17"/>
@@ -5172,7 +5983,7 @@
       <c r="T24" s="21"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="49"/>
+      <c r="B25" s="45"/>
       <c r="C25" s="11"/>
       <c r="D25" s="21"/>
       <c r="E25" s="17"/>
@@ -5193,7 +6004,7 @@
       <c r="T25" s="21"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="49"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="11"/>
       <c r="D26" s="21"/>
       <c r="E26" s="17"/>
@@ -5214,7 +6025,7 @@
       <c r="T26" s="21"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B27" s="49"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="11"/>
       <c r="D27" s="21"/>
       <c r="E27" s="17"/>
@@ -5235,7 +6046,7 @@
       <c r="T27" s="21"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="49"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="11"/>
       <c r="D28" s="21"/>
       <c r="E28" s="17"/>
@@ -5294,8 +6105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1AACEDC-A0D0-42F4-BC04-689F8C4AA144}">
   <dimension ref="B2:T36"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5310,48 +6121,48 @@
         <f>B18</f>
         <v>0</v>
       </c>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="56">
         <f>B27</f>
         <v>0.5</v>
       </c>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="47"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="49"/>
       <c r="N3" s="56">
         <v>1</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
-      <c r="Q3" s="47"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
     </row>
     <row r="4" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="43" t="s">
+      <c r="G4" s="51"/>
+      <c r="H4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="44"/>
-      <c r="J4" s="43" t="s">
+      <c r="I4" s="51"/>
+      <c r="J4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="43" t="s">
+      <c r="K4" s="51"/>
+      <c r="L4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="44"/>
-      <c r="N4" s="43" t="s">
+      <c r="M4" s="51"/>
+      <c r="N4" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="43" t="s">
+      <c r="O4" s="51"/>
+      <c r="P4" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="44"/>
+      <c r="Q4" s="51"/>
     </row>
     <row r="5" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -5401,7 +6212,7 @@
       </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="44" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -5463,7 +6274,7 @@
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="49"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="19" t="s">
         <v>13</v>
       </c>
@@ -5523,7 +6334,7 @@
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="19" t="s">
         <v>14</v>
       </c>
@@ -5583,7 +6394,7 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="49"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="19" t="s">
         <v>8</v>
       </c>
@@ -5643,7 +6454,7 @@
       </c>
     </row>
     <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="50"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="30" t="s">
         <v>15</v>
       </c>
@@ -5776,18 +6587,18 @@
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="44"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="51"/>
     </row>
     <row r="17" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="25"/>
@@ -5830,20 +6641,20 @@
       <c r="O17" s="2">
         <v>10</v>
       </c>
-      <c r="P17" s="43" t="s">
+      <c r="P17" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="43" t="s">
+      <c r="Q17" s="51"/>
+      <c r="R17" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S17" s="44"/>
+      <c r="S17" s="51"/>
       <c r="T17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:20" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="52">
+      <c r="B18" s="53">
         <v>0</v>
       </c>
       <c r="C18" s="18" t="str">
@@ -5900,7 +6711,7 @@
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="53"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="19" t="str">
         <f t="shared" ref="C19:E19" si="11">C7</f>
         <v>F1_g-6</v>
@@ -5955,7 +6766,7 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="53"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="19" t="str">
         <f t="shared" ref="C20:E20" si="17">C8</f>
         <v>Beijing-3</v>
@@ -6010,7 +6821,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="53"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="19" t="str">
         <f t="shared" ref="C21:E21" si="18">C9</f>
         <v>Hefei-10</v>
@@ -6114,7 +6925,7 @@
         <f t="shared" si="15"/>
         <v>1.278494049175305E-2</v>
       </c>
-      <c r="T22" s="54">
+      <c r="T22" s="43">
         <f t="shared" si="16"/>
         <v>4205.6451871264653</v>
       </c>
@@ -6123,18 +6934,18 @@
     <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="26"/>
-      <c r="F25" s="43" t="s">
+      <c r="F25" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="44"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="51"/>
     </row>
     <row r="26" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11"/>
@@ -6177,20 +6988,20 @@
       <c r="O26" s="2">
         <v>10</v>
       </c>
-      <c r="P26" s="43" t="s">
+      <c r="P26" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="Q26" s="44"/>
-      <c r="R26" s="43" t="s">
+      <c r="Q26" s="51"/>
+      <c r="R26" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="S26" s="44"/>
+      <c r="S26" s="51"/>
       <c r="T26" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="52">
+      <c r="B27" s="53">
         <v>0.5</v>
       </c>
       <c r="C27" s="18" t="str">
@@ -6247,7 +7058,7 @@
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="53"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="19" t="str">
         <f t="shared" ref="C28:E28" si="21">C7</f>
         <v>F1_g-6</v>
@@ -6302,7 +7113,7 @@
       </c>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B29" s="53"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="19" t="str">
         <f t="shared" ref="C29:E29" si="27">C8</f>
         <v>Beijing-3</v>
@@ -6357,7 +7168,7 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="53"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="19" t="str">
         <f t="shared" ref="C30:E30" si="28">C9</f>
         <v>Hefei-10</v>
@@ -6461,7 +7272,7 @@
         <f t="shared" si="25"/>
         <v>7.7280012731468783E-3</v>
       </c>
-      <c r="T31" s="54">
+      <c r="T31" s="43">
         <f t="shared" si="26"/>
         <v>4877.857726502486</v>
       </c>
@@ -6558,11 +7369,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="F25:O25"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="N3:Q3"/>
@@ -6570,27 +7380,28 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B27:B31"/>
     <mergeCell ref="F16:O16"/>
     <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="F25:O25"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="R26:S26"/>
   </mergeCells>
   <conditionalFormatting sqref="G9 K9 O9">
-    <cfRule type="top10" dxfId="24" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="144" priority="4" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 K10 O10">
-    <cfRule type="top10" dxfId="23" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="143" priority="5" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8 K8 O8">
-    <cfRule type="top10" dxfId="22" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="142" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7 K7 O7">
-    <cfRule type="top10" dxfId="21" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="141" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6 K6 O6">
-    <cfRule type="top10" dxfId="20" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="140" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6598,72 +7409,1478 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB94F69-007F-4C31-B54F-A9483762C616}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:T49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="56">
+        <f>B18</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="56">
+        <f>B27</f>
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="49"/>
+    </row>
+    <row r="4" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="51"/>
+      <c r="H4" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="51"/>
+      <c r="J4" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="51"/>
+      <c r="L4" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="51"/>
+      <c r="N4" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="51"/>
+      <c r="P4" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="51"/>
+    </row>
+    <row r="5" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="10">
+        <v>375</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1602229</v>
+      </c>
+      <c r="F6" s="23">
+        <f>P18</f>
+        <v>1612530</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" ref="G6:I10" si="0">Q18</f>
+        <v>6.429168364821658E-3</v>
+      </c>
+      <c r="H6" s="23">
+        <f t="shared" si="0"/>
+        <v>1618795.6</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" si="0"/>
+        <v>1.0339720476910674E-2</v>
+      </c>
+      <c r="J6" s="23">
+        <f>P27</f>
+        <v>1613111</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" ref="K6:M10" si="1">Q27</f>
+        <v>6.7917881900776411E-3</v>
+      </c>
+      <c r="L6" s="23">
+        <f t="shared" si="1"/>
+        <v>1615329</v>
+      </c>
+      <c r="M6" s="12">
+        <f t="shared" si="1"/>
+        <v>8.1761096572336989E-3</v>
+      </c>
+      <c r="N6" s="23">
+        <f>Comparison!N6</f>
+        <v>1615420</v>
+      </c>
+      <c r="O6" s="14">
+        <f>Comparison!O6</f>
+        <v>8.2329055334786627E-3</v>
+      </c>
+      <c r="P6" s="23">
+        <f>Comparison!P6</f>
+        <v>1621760.4</v>
+      </c>
+      <c r="Q6" s="12">
+        <f>Comparison!Q6</f>
+        <v>1.2190142607579668E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="45"/>
+      <c r="C7" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="11">
+        <v>780</v>
+      </c>
+      <c r="E7" s="17">
+        <v>474809</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" ref="F7:F10" si="2">P19</f>
+        <v>438422</v>
+      </c>
+      <c r="G7" s="15">
+        <f t="shared" si="0"/>
+        <v>-7.6635025873561746E-2</v>
+      </c>
+      <c r="H7" s="22">
+        <f t="shared" si="0"/>
+        <v>440105.4</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>-7.3089600239254038E-2</v>
+      </c>
+      <c r="J7" s="22">
+        <f t="shared" ref="J7:J10" si="3">P28</f>
+        <v>439328</v>
+      </c>
+      <c r="K7" s="15">
+        <f t="shared" si="1"/>
+        <v>-7.4726890181104455E-2</v>
+      </c>
+      <c r="L7" s="22">
+        <f t="shared" si="1"/>
+        <v>440381.6</v>
+      </c>
+      <c r="M7" s="13">
+        <f t="shared" si="1"/>
+        <v>-7.2507892647359351E-2</v>
+      </c>
+      <c r="N7" s="22">
+        <f>Comparison!N7</f>
+        <v>439830</v>
+      </c>
+      <c r="O7" s="15">
+        <f>Comparison!O7</f>
+        <v>-7.3669622943120294E-2</v>
+      </c>
+      <c r="P7" s="22">
+        <f>Comparison!P7</f>
+        <v>441952.2</v>
+      </c>
+      <c r="Q7" s="13">
+        <f>Comparison!Q7</f>
+        <v>-6.9200036225092632E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="45"/>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1075</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1534878</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="2"/>
+        <v>1539963</v>
+      </c>
+      <c r="G8" s="15">
+        <f t="shared" si="0"/>
+        <v>3.3129668937856849E-3</v>
+      </c>
+      <c r="H8" s="22">
+        <f t="shared" si="0"/>
+        <v>1546492.6</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="0"/>
+        <v>7.5671160834933637E-3</v>
+      </c>
+      <c r="J8" s="22">
+        <f t="shared" si="3"/>
+        <v>1544811</v>
+      </c>
+      <c r="K8" s="15">
+        <f t="shared" si="1"/>
+        <v>6.4715241211352748E-3</v>
+      </c>
+      <c r="L8" s="22">
+        <f t="shared" si="1"/>
+        <v>1551337.4</v>
+      </c>
+      <c r="M8" s="13">
+        <f t="shared" si="1"/>
+        <v>1.0723588454587318E-2</v>
+      </c>
+      <c r="N8" s="22">
+        <f>Comparison!N8</f>
+        <v>1540668</v>
+      </c>
+      <c r="O8" s="15">
+        <f>Comparison!O8</f>
+        <v>3.7722867876144317E-3</v>
+      </c>
+      <c r="P8" s="22">
+        <f>Comparison!P8</f>
+        <v>1543291.1</v>
+      </c>
+      <c r="Q8" s="13">
+        <f>Comparison!Q8</f>
+        <v>5.4812825514471974E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="45"/>
+      <c r="C9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1212</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1748829</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="2"/>
+        <v>1754557</v>
+      </c>
+      <c r="G9" s="15">
+        <f t="shared" si="0"/>
+        <v>3.2753345238443199E-3</v>
+      </c>
+      <c r="H9" s="22">
+        <f t="shared" si="0"/>
+        <v>1761429</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>7.2048210545456737E-3</v>
+      </c>
+      <c r="J9" s="22">
+        <f t="shared" si="3"/>
+        <v>1755539</v>
+      </c>
+      <c r="K9" s="15">
+        <f t="shared" si="1"/>
+        <v>3.8368531171428799E-3</v>
+      </c>
+      <c r="L9" s="22">
+        <f t="shared" si="1"/>
+        <v>1761406</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" si="1"/>
+        <v>7.1916693970650591E-3</v>
+      </c>
+      <c r="N9" s="22">
+        <f>Comparison!N9</f>
+        <v>1757911</v>
+      </c>
+      <c r="O9" s="15">
+        <f>Comparison!O9</f>
+        <v>5.1931892712209216E-3</v>
+      </c>
+      <c r="P9" s="22">
+        <f>Comparison!P9</f>
+        <v>1765520.7</v>
+      </c>
+      <c r="Q9" s="13">
+        <f>Comparison!Q9</f>
+        <v>9.5445009203301012E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="46"/>
+      <c r="C10" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="24">
+        <v>1792</v>
+      </c>
+      <c r="E10" s="31">
+        <v>2199275</v>
+      </c>
+      <c r="F10" s="32">
+        <f t="shared" si="2"/>
+        <v>2205729</v>
+      </c>
+      <c r="G10" s="33">
+        <f t="shared" si="0"/>
+        <v>2.9346034488637596E-3</v>
+      </c>
+      <c r="H10" s="32">
+        <f t="shared" si="0"/>
+        <v>2213915.4</v>
+      </c>
+      <c r="I10" s="34">
+        <f t="shared" si="0"/>
+        <v>6.6569210307942939E-3</v>
+      </c>
+      <c r="J10" s="32">
+        <f t="shared" si="3"/>
+        <v>2202401</v>
+      </c>
+      <c r="K10" s="33">
+        <f t="shared" si="1"/>
+        <v>1.4213774994031869E-3</v>
+      </c>
+      <c r="L10" s="32">
+        <f t="shared" si="1"/>
+        <v>2209938.4</v>
+      </c>
+      <c r="M10" s="34">
+        <f t="shared" si="1"/>
+        <v>4.8485978333767665E-3</v>
+      </c>
+      <c r="N10" s="32">
+        <f>Comparison!N10</f>
+        <v>2204970</v>
+      </c>
+      <c r="O10" s="33">
+        <f>Comparison!O10</f>
+        <v>2.5894897182026089E-3</v>
+      </c>
+      <c r="P10" s="32">
+        <f>Comparison!P10</f>
+        <v>2215325.7000000002</v>
+      </c>
+      <c r="Q10" s="34">
+        <f>Comparison!Q10</f>
+        <v>7.2981778085960958E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="27"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="29"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="27"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="29"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="27"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="29"/>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="27"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="29"/>
+    </row>
+    <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="2:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="51"/>
+    </row>
+    <row r="17" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="25"/>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4">
+        <v>3</v>
+      </c>
+      <c r="I17" s="4">
+        <v>4</v>
+      </c>
+      <c r="J17" s="4">
+        <v>5</v>
+      </c>
+      <c r="K17" s="4">
+        <v>6</v>
+      </c>
+      <c r="L17" s="4">
+        <v>7</v>
+      </c>
+      <c r="M17" s="4">
+        <v>8</v>
+      </c>
+      <c r="N17" s="4">
+        <v>9</v>
+      </c>
+      <c r="O17" s="2">
+        <v>10</v>
+      </c>
+      <c r="P17" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" s="51"/>
+      <c r="T17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="53">
+        <v>0</v>
+      </c>
+      <c r="C18" s="18" t="str">
+        <f>C6</f>
+        <v>egl-g2-E</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" ref="D18:E18" si="4">D6</f>
+        <v>375</v>
+      </c>
+      <c r="E18" s="16">
+        <f t="shared" si="4"/>
+        <v>1602229</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1612530</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1621726</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1618473</v>
+      </c>
+      <c r="I18" s="5">
+        <v>1620487</v>
+      </c>
+      <c r="J18" s="23">
+        <v>1620762</v>
+      </c>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="5">
+        <f>MIN(F18:O18)</f>
+        <v>1612530</v>
+      </c>
+      <c r="Q18" s="13">
+        <f>P18/E18-1</f>
+        <v>6.429168364821658E-3</v>
+      </c>
+      <c r="R18" s="5">
+        <f>AVERAGE(F18:O18)</f>
+        <v>1618795.6</v>
+      </c>
+      <c r="S18" s="13">
+        <f>R18/E18-1</f>
+        <v>1.0339720476910674E-2</v>
+      </c>
+      <c r="T18" s="21">
+        <f>_xlfn.STDEV.P(F18:O18)</f>
+        <v>3306.8601784774633</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="19" t="str">
+        <f t="shared" ref="C19:E22" si="5">C7</f>
+        <v>F1_g-6</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="5"/>
+        <v>780</v>
+      </c>
+      <c r="E19" s="17">
+        <f t="shared" si="5"/>
+        <v>474809</v>
+      </c>
+      <c r="F19" s="5">
+        <v>438422</v>
+      </c>
+      <c r="G19" s="5">
+        <v>439556</v>
+      </c>
+      <c r="H19" s="5">
+        <v>440640</v>
+      </c>
+      <c r="I19" s="5">
+        <v>440996</v>
+      </c>
+      <c r="J19" s="22">
+        <v>440913</v>
+      </c>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="5">
+        <f t="shared" ref="P19:P22" si="6">MIN(F19:O19)</f>
+        <v>438422</v>
+      </c>
+      <c r="Q19" s="13">
+        <f t="shared" ref="Q19:Q22" si="7">P19/E19-1</f>
+        <v>-7.6635025873561746E-2</v>
+      </c>
+      <c r="R19" s="5">
+        <f t="shared" ref="R19:R22" si="8">AVERAGE(F19:O19)</f>
+        <v>440105.4</v>
+      </c>
+      <c r="S19" s="13">
+        <f t="shared" ref="S19:S22" si="9">R19/E19-1</f>
+        <v>-7.3089600239254038E-2</v>
+      </c>
+      <c r="T19" s="21">
+        <f t="shared" ref="T19:T22" si="10">_xlfn.STDEV.P(F19:O19)</f>
+        <v>986.5960875657272</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>Beijing-3</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="5"/>
+        <v>1075</v>
+      </c>
+      <c r="E20" s="17">
+        <f t="shared" si="5"/>
+        <v>1534878</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1545043</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1539963</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1542107</v>
+      </c>
+      <c r="I20" s="5">
+        <v>1555455</v>
+      </c>
+      <c r="J20" s="22">
+        <v>1549895</v>
+      </c>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="5">
+        <f t="shared" si="6"/>
+        <v>1539963</v>
+      </c>
+      <c r="Q20" s="13">
+        <f t="shared" si="7"/>
+        <v>3.3129668937856849E-3</v>
+      </c>
+      <c r="R20" s="5">
+        <f t="shared" si="8"/>
+        <v>1546492.6</v>
+      </c>
+      <c r="S20" s="13">
+        <f t="shared" si="9"/>
+        <v>7.5671160834933637E-3</v>
+      </c>
+      <c r="T20" s="21">
+        <f t="shared" si="10"/>
+        <v>5583.3940072325186</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="54"/>
+      <c r="C21" s="19" t="str">
+        <f t="shared" si="5"/>
+        <v>Hefei-10</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="5"/>
+        <v>1212</v>
+      </c>
+      <c r="E21" s="17">
+        <f t="shared" si="5"/>
+        <v>1748829</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1754557</v>
+      </c>
+      <c r="G21" s="5">
+        <v>1764297</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1761706</v>
+      </c>
+      <c r="I21" s="5">
+        <v>1760685</v>
+      </c>
+      <c r="J21" s="22">
+        <v>1765900</v>
+      </c>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="5">
+        <f t="shared" si="6"/>
+        <v>1754557</v>
+      </c>
+      <c r="Q21" s="13">
+        <f t="shared" si="7"/>
+        <v>3.2753345238443199E-3</v>
+      </c>
+      <c r="R21" s="5">
+        <f t="shared" si="8"/>
+        <v>1761429</v>
+      </c>
+      <c r="S21" s="13">
+        <f t="shared" si="9"/>
+        <v>7.2048210545456737E-3</v>
+      </c>
+      <c r="T21" s="21">
+        <f t="shared" si="10"/>
+        <v>3900.5105819623154</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="55"/>
+      <c r="C22" s="30" t="str">
+        <f t="shared" si="5"/>
+        <v>Beijing-5</v>
+      </c>
+      <c r="D22" s="24">
+        <f t="shared" si="5"/>
+        <v>1792</v>
+      </c>
+      <c r="E22" s="31">
+        <f t="shared" si="5"/>
+        <v>2199275</v>
+      </c>
+      <c r="F22" s="32">
+        <v>2205729</v>
+      </c>
+      <c r="G22" s="32">
+        <v>2219628</v>
+      </c>
+      <c r="H22" s="32">
+        <v>2219855</v>
+      </c>
+      <c r="I22" s="32">
+        <v>2209528</v>
+      </c>
+      <c r="J22" s="32">
+        <v>2214837</v>
+      </c>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="31"/>
+      <c r="P22" s="32">
+        <f t="shared" si="6"/>
+        <v>2205729</v>
+      </c>
+      <c r="Q22" s="34">
+        <f t="shared" si="7"/>
+        <v>2.9346034488637596E-3</v>
+      </c>
+      <c r="R22" s="32">
+        <f t="shared" si="8"/>
+        <v>2213915.4</v>
+      </c>
+      <c r="S22" s="34">
+        <f t="shared" si="9"/>
+        <v>6.6569210307942939E-3</v>
+      </c>
+      <c r="T22" s="43">
+        <f t="shared" si="10"/>
+        <v>5568.2747274178209</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="26"/>
+      <c r="F25" s="50" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="52"/>
+      <c r="O25" s="51"/>
+    </row>
+    <row r="26" spans="2:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="4">
+        <v>2</v>
+      </c>
+      <c r="H26" s="4">
+        <v>3</v>
+      </c>
+      <c r="I26" s="4">
+        <v>4</v>
+      </c>
+      <c r="J26" s="4">
+        <v>5</v>
+      </c>
+      <c r="K26" s="4">
+        <v>6</v>
+      </c>
+      <c r="L26" s="4">
+        <v>7</v>
+      </c>
+      <c r="M26" s="4">
+        <v>8</v>
+      </c>
+      <c r="N26" s="4">
+        <v>9</v>
+      </c>
+      <c r="O26" s="2">
+        <v>10</v>
+      </c>
+      <c r="P26" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="50" t="s">
+        <v>3</v>
+      </c>
+      <c r="S26" s="51"/>
+      <c r="T26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="53">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="18" t="str">
+        <f>C6</f>
+        <v>egl-g2-E</v>
+      </c>
+      <c r="D27" s="10">
+        <f t="shared" ref="D27:E27" si="11">D6</f>
+        <v>375</v>
+      </c>
+      <c r="E27" s="16">
+        <f t="shared" si="11"/>
+        <v>1602229</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1613975</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1613966</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1622120</v>
+      </c>
+      <c r="I27" s="5">
+        <v>1613111</v>
+      </c>
+      <c r="J27" s="23">
+        <v>1613473</v>
+      </c>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="5">
+        <f>MIN(F27:O27)</f>
+        <v>1613111</v>
+      </c>
+      <c r="Q27" s="13">
+        <f>P27/E27-1</f>
+        <v>6.7917881900776411E-3</v>
+      </c>
+      <c r="R27" s="5">
+        <f>AVERAGE(F27:O27)</f>
+        <v>1615329</v>
+      </c>
+      <c r="S27" s="13">
+        <f>R27/E27-1</f>
+        <v>8.1761096572336989E-3</v>
+      </c>
+      <c r="T27" s="21">
+        <f>_xlfn.STDEV.P(F27:O27)</f>
+        <v>3410.9537082757365</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="54"/>
+      <c r="C28" s="19" t="str">
+        <f t="shared" ref="C28:E31" si="12">C7</f>
+        <v>F1_g-6</v>
+      </c>
+      <c r="D28" s="11">
+        <f t="shared" si="12"/>
+        <v>780</v>
+      </c>
+      <c r="E28" s="17">
+        <f t="shared" si="12"/>
+        <v>474809</v>
+      </c>
+      <c r="F28" s="5">
+        <v>440199</v>
+      </c>
+      <c r="G28" s="5">
+        <v>441627</v>
+      </c>
+      <c r="H28" s="5">
+        <v>439332</v>
+      </c>
+      <c r="I28" s="5">
+        <v>441422</v>
+      </c>
+      <c r="J28" s="22">
+        <v>439328</v>
+      </c>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="5">
+        <f t="shared" ref="P28:P31" si="13">MIN(F28:O28)</f>
+        <v>439328</v>
+      </c>
+      <c r="Q28" s="13">
+        <f t="shared" ref="Q28:Q31" si="14">P28/E28-1</f>
+        <v>-7.4726890181104455E-2</v>
+      </c>
+      <c r="R28" s="5">
+        <f t="shared" ref="R28:R31" si="15">AVERAGE(F28:O28)</f>
+        <v>440381.6</v>
+      </c>
+      <c r="S28" s="13">
+        <f t="shared" ref="S28:S31" si="16">R28/E28-1</f>
+        <v>-7.2507892647359351E-2</v>
+      </c>
+      <c r="T28" s="21">
+        <f t="shared" ref="T28:T31" si="17">_xlfn.STDEV.P(F28:O28)</f>
+        <v>987.77823422061692</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="54"/>
+      <c r="C29" s="19" t="str">
+        <f t="shared" si="12"/>
+        <v>Beijing-3</v>
+      </c>
+      <c r="D29" s="11">
+        <f t="shared" si="12"/>
+        <v>1075</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" si="12"/>
+        <v>1534878</v>
+      </c>
+      <c r="F29" s="22">
+        <v>1544811</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1545911</v>
+      </c>
+      <c r="H29" s="22">
+        <v>1557121</v>
+      </c>
+      <c r="I29" s="22">
+        <v>1554298</v>
+      </c>
+      <c r="J29" s="22">
+        <v>1554546</v>
+      </c>
+      <c r="K29" s="22"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="5">
+        <f t="shared" si="13"/>
+        <v>1544811</v>
+      </c>
+      <c r="Q29" s="13">
+        <f t="shared" si="14"/>
+        <v>6.4715241211352748E-3</v>
+      </c>
+      <c r="R29" s="5">
+        <f t="shared" si="15"/>
+        <v>1551337.4</v>
+      </c>
+      <c r="S29" s="13">
+        <f t="shared" si="16"/>
+        <v>1.0723588454587318E-2</v>
+      </c>
+      <c r="T29" s="21">
+        <f t="shared" si="17"/>
+        <v>4990.9920697192056</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="54"/>
+      <c r="C30" s="19" t="str">
+        <f t="shared" si="12"/>
+        <v>Hefei-10</v>
+      </c>
+      <c r="D30" s="11">
+        <f t="shared" si="12"/>
+        <v>1212</v>
+      </c>
+      <c r="E30" s="17">
+        <f t="shared" si="12"/>
+        <v>1748829</v>
+      </c>
+      <c r="F30" s="22">
+        <v>1755539</v>
+      </c>
+      <c r="G30" s="22">
+        <v>1760969</v>
+      </c>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22">
+        <v>1764796</v>
+      </c>
+      <c r="J30" s="22">
+        <v>1764320</v>
+      </c>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="5">
+        <f t="shared" si="13"/>
+        <v>1755539</v>
+      </c>
+      <c r="Q30" s="13">
+        <f t="shared" si="14"/>
+        <v>3.8368531171428799E-3</v>
+      </c>
+      <c r="R30" s="5">
+        <f t="shared" si="15"/>
+        <v>1761406</v>
+      </c>
+      <c r="S30" s="13">
+        <f t="shared" si="16"/>
+        <v>7.1916693970650591E-3</v>
+      </c>
+      <c r="T30" s="21">
+        <f t="shared" si="17"/>
+        <v>3694.46051542035</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="55"/>
+      <c r="C31" s="30" t="str">
+        <f t="shared" si="12"/>
+        <v>Beijing-5</v>
+      </c>
+      <c r="D31" s="24">
+        <f t="shared" si="12"/>
+        <v>1792</v>
+      </c>
+      <c r="E31" s="31">
+        <f t="shared" si="12"/>
+        <v>2199275</v>
+      </c>
+      <c r="F31" s="32">
+        <v>2208944</v>
+      </c>
+      <c r="G31" s="32">
+        <v>2202401</v>
+      </c>
+      <c r="H31" s="32">
+        <v>2205117</v>
+      </c>
+      <c r="I31" s="32">
+        <v>2227335</v>
+      </c>
+      <c r="J31" s="32">
+        <v>2205895</v>
+      </c>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="32">
+        <f t="shared" si="13"/>
+        <v>2202401</v>
+      </c>
+      <c r="Q31" s="34">
+        <f t="shared" si="14"/>
+        <v>1.4213774994031869E-3</v>
+      </c>
+      <c r="R31" s="32">
+        <f t="shared" si="15"/>
+        <v>2209938.4</v>
+      </c>
+      <c r="S31" s="34">
+        <f t="shared" si="16"/>
+        <v>4.8485978333767665E-3</v>
+      </c>
+      <c r="T31" s="43">
+        <f t="shared" si="17"/>
+        <v>8944.6956706195433</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>1545043</v>
+      </c>
+      <c r="F39">
+        <v>1539963</v>
+      </c>
+      <c r="G39">
+        <v>1542107</v>
+      </c>
+      <c r="H39">
+        <v>1555455</v>
+      </c>
+      <c r="I39">
+        <v>1549895</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>2205729</v>
+      </c>
+      <c r="F40">
+        <v>2219628</v>
+      </c>
+      <c r="G40">
+        <v>2219855</v>
+      </c>
+      <c r="H40">
+        <v>2209528</v>
+      </c>
+      <c r="I40">
+        <v>2214837</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>1612530</v>
+      </c>
+      <c r="F41">
+        <v>1621726</v>
+      </c>
+      <c r="G41">
+        <v>1618473</v>
+      </c>
+      <c r="H41">
+        <v>1620487</v>
+      </c>
+      <c r="I41">
+        <v>1620762</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>438422</v>
+      </c>
+      <c r="F42">
+        <v>439556</v>
+      </c>
+      <c r="G42">
+        <v>440640</v>
+      </c>
+      <c r="H42">
+        <v>440996</v>
+      </c>
+      <c r="I42">
+        <v>440913</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>1754557</v>
+      </c>
+      <c r="F43">
+        <v>1764297</v>
+      </c>
+      <c r="G43">
+        <v>1761706</v>
+      </c>
+      <c r="H43">
+        <v>1760685</v>
+      </c>
+      <c r="I43">
+        <v>1765900</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45">
+        <v>1544811</v>
+      </c>
+      <c r="F45">
+        <v>1545911</v>
+      </c>
+      <c r="G45">
+        <v>1557121</v>
+      </c>
+      <c r="H45">
+        <v>1554298</v>
+      </c>
+      <c r="I45">
+        <v>1554546</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46">
+        <v>2208944</v>
+      </c>
+      <c r="F46">
+        <v>2202401</v>
+      </c>
+      <c r="G46">
+        <v>2205117</v>
+      </c>
+      <c r="H46">
+        <v>2227335</v>
+      </c>
+      <c r="I46">
+        <v>2205895</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47">
+        <v>1613975</v>
+      </c>
+      <c r="F47">
+        <v>1613966</v>
+      </c>
+      <c r="G47">
+        <v>1622120</v>
+      </c>
+      <c r="H47">
+        <v>1613111</v>
+      </c>
+      <c r="I47">
+        <v>1613473</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48">
+        <v>440199</v>
+      </c>
+      <c r="F48">
+        <v>441627</v>
+      </c>
+      <c r="G48">
+        <v>439332</v>
+      </c>
+      <c r="H48">
+        <v>441422</v>
+      </c>
+      <c r="I48">
+        <v>439328</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <v>1755539</v>
+      </c>
+      <c r="F49">
+        <v>1760969</v>
+      </c>
+      <c r="H49">
+        <v>1764796</v>
+      </c>
+      <c r="I49">
+        <v>1764320</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="F16:O16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F25:O25"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="N4:O4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="G9 K9 O9">
+    <cfRule type="top10" dxfId="4" priority="4" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10 K10 O10">
+    <cfRule type="top10" dxfId="3" priority="5" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8 K8 O8">
+    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7 K7 O7">
+    <cfRule type="top10" dxfId="1" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6 K6 O6">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACEBDDF-2E4A-43BA-9C94-A9709F6384C0}">
-  <dimension ref="C13:Q36"/>
+  <dimension ref="C13:Q62"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:H36"/>
+    <sheetView topLeftCell="A39" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="13" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="3:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="45" t="s">
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="45" t="s">
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="47"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="49"/>
     </row>
     <row r="15" spans="3:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="43" t="s">
+      <c r="G15" s="51"/>
+      <c r="H15" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="44"/>
-      <c r="J15" s="43" t="s">
+      <c r="I15" s="51"/>
+      <c r="J15" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="43" t="s">
+      <c r="K15" s="51"/>
+      <c r="L15" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="44"/>
-      <c r="N15" s="43" t="s">
+      <c r="M15" s="51"/>
+      <c r="N15" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="O15" s="44"/>
-      <c r="P15" s="43" t="s">
+      <c r="O15" s="51"/>
+      <c r="P15" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="44"/>
+      <c r="Q15" s="51"/>
     </row>
     <row r="16" spans="3:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
@@ -6952,9 +9169,6 @@
       <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="J25" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="26" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
@@ -6975,24 +9189,6 @@
       <c r="H26">
         <v>1542186</v>
       </c>
-      <c r="J26" t="s">
-        <v>14</v>
-      </c>
-      <c r="K26">
-        <v>1543703</v>
-      </c>
-      <c r="L26">
-        <v>1544972</v>
-      </c>
-      <c r="M26">
-        <v>1547652</v>
-      </c>
-      <c r="N26">
-        <v>1549337</v>
-      </c>
-      <c r="O26">
-        <v>1544930</v>
-      </c>
     </row>
     <row r="27" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
@@ -7013,24 +9209,6 @@
       <c r="H27">
         <v>1617052</v>
       </c>
-      <c r="J27" t="s">
-        <v>8</v>
-      </c>
-      <c r="K27">
-        <v>1776990</v>
-      </c>
-      <c r="L27">
-        <v>1772324</v>
-      </c>
-      <c r="M27">
-        <v>1770664</v>
-      </c>
-      <c r="N27">
-        <v>1768517</v>
-      </c>
-      <c r="O27">
-        <v>1778238</v>
-      </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
@@ -7051,24 +9229,6 @@
       <c r="H28">
         <v>2212731</v>
       </c>
-      <c r="J28" t="s">
-        <v>13</v>
-      </c>
-      <c r="K28">
-        <v>444906</v>
-      </c>
-      <c r="L28">
-        <v>445548</v>
-      </c>
-      <c r="M28">
-        <v>444660</v>
-      </c>
-      <c r="N28">
-        <v>444008</v>
-      </c>
-      <c r="O28">
-        <v>444983</v>
-      </c>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
@@ -7089,24 +9249,6 @@
       <c r="H29">
         <v>1754102</v>
       </c>
-      <c r="J29" t="s">
-        <v>15</v>
-      </c>
-      <c r="K29">
-        <v>2227071</v>
-      </c>
-      <c r="L29">
-        <v>2228918</v>
-      </c>
-      <c r="M29">
-        <v>2230846</v>
-      </c>
-      <c r="N29">
-        <v>2219441</v>
-      </c>
-      <c r="O29">
-        <v>2230687</v>
-      </c>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
@@ -7127,32 +9269,11 @@
       <c r="H30">
         <v>442640</v>
       </c>
-      <c r="J30" t="s">
-        <v>7</v>
-      </c>
-      <c r="K30">
-        <v>1621652</v>
-      </c>
-      <c r="L30">
-        <v>1634999</v>
-      </c>
-      <c r="M30">
-        <v>1633269</v>
-      </c>
-      <c r="N30">
-        <v>1624684</v>
-      </c>
-      <c r="O30">
-        <v>1620274</v>
-      </c>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="J31" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="32" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
@@ -7173,26 +9294,8 @@
       <c r="H32">
         <v>1543609</v>
       </c>
-      <c r="J32" t="s">
-        <v>14</v>
-      </c>
-      <c r="K32">
-        <v>1546255</v>
-      </c>
-      <c r="L32">
-        <v>1545396</v>
-      </c>
-      <c r="M32">
-        <v>1545481</v>
-      </c>
-      <c r="N32">
-        <v>1549060</v>
-      </c>
-      <c r="O32">
-        <v>1548049</v>
-      </c>
-    </row>
-    <row r="33" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>7</v>
       </c>
@@ -7211,26 +9314,8 @@
       <c r="H33">
         <v>1618552</v>
       </c>
-      <c r="J33" t="s">
-        <v>8</v>
-      </c>
-      <c r="K33">
-        <v>1767092</v>
-      </c>
-      <c r="L33">
-        <v>1768499</v>
-      </c>
-      <c r="M33">
-        <v>1760107</v>
-      </c>
-      <c r="N33">
-        <v>1762926</v>
-      </c>
-      <c r="O33">
-        <v>1759054</v>
-      </c>
-    </row>
-    <row r="34" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>15</v>
       </c>
@@ -7249,26 +9334,8 @@
       <c r="H34">
         <v>2197230</v>
       </c>
-      <c r="J34" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34">
-        <v>441529</v>
-      </c>
-      <c r="L34">
-        <v>438336</v>
-      </c>
-      <c r="M34">
-        <v>440769</v>
-      </c>
-      <c r="N34">
-        <v>441688</v>
-      </c>
-      <c r="O34">
-        <v>439772</v>
-      </c>
-    </row>
-    <row r="35" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>8</v>
       </c>
@@ -7287,26 +9354,8 @@
       <c r="H35">
         <v>1753014</v>
       </c>
-      <c r="J35" t="s">
-        <v>15</v>
-      </c>
-      <c r="K35">
-        <v>2222391</v>
-      </c>
-      <c r="L35">
-        <v>2209445</v>
-      </c>
-      <c r="M35">
-        <v>2211693</v>
-      </c>
-      <c r="N35">
-        <v>2218899</v>
-      </c>
-      <c r="O35">
-        <v>2218927</v>
-      </c>
-    </row>
-    <row r="36" spans="3:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>13</v>
       </c>
@@ -7325,23 +9374,422 @@
       <c r="H36">
         <v>439013</v>
       </c>
-      <c r="J36" t="s">
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>1543703</v>
+      </c>
+      <c r="E40">
+        <v>1544972</v>
+      </c>
+      <c r="F40">
+        <v>1547652</v>
+      </c>
+      <c r="G40">
+        <v>1549337</v>
+      </c>
+      <c r="H40">
+        <v>1544930</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>2227071</v>
+      </c>
+      <c r="E41">
+        <v>2228918</v>
+      </c>
+      <c r="F41">
+        <v>2230846</v>
+      </c>
+      <c r="G41">
+        <v>2219441</v>
+      </c>
+      <c r="H41">
+        <v>2230687</v>
+      </c>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="K36">
+      <c r="D42">
+        <v>1621652</v>
+      </c>
+      <c r="E42">
+        <v>1634999</v>
+      </c>
+      <c r="F42">
+        <v>1633269</v>
+      </c>
+      <c r="G42">
+        <v>1624684</v>
+      </c>
+      <c r="H42">
+        <v>1620274</v>
+      </c>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>444906</v>
+      </c>
+      <c r="E43">
+        <v>445548</v>
+      </c>
+      <c r="F43">
+        <v>444660</v>
+      </c>
+      <c r="G43">
+        <v>444008</v>
+      </c>
+      <c r="H43">
+        <v>444983</v>
+      </c>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>1776990</v>
+      </c>
+      <c r="E44">
+        <v>1772324</v>
+      </c>
+      <c r="F44">
+        <v>1770664</v>
+      </c>
+      <c r="G44">
+        <v>1768517</v>
+      </c>
+      <c r="H44">
+        <v>1778238</v>
+      </c>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>1546255</v>
+      </c>
+      <c r="E46">
+        <v>1545396</v>
+      </c>
+      <c r="F46">
+        <v>1545481</v>
+      </c>
+      <c r="G46">
+        <v>1549060</v>
+      </c>
+      <c r="H46">
+        <v>1548049</v>
+      </c>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47">
+        <v>2222391</v>
+      </c>
+      <c r="E47">
+        <v>2209445</v>
+      </c>
+      <c r="F47">
+        <v>2211693</v>
+      </c>
+      <c r="G47">
+        <v>2218899</v>
+      </c>
+      <c r="H47">
+        <v>2218927</v>
+      </c>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48">
         <v>1623446</v>
       </c>
-      <c r="L36">
+      <c r="E48">
         <v>1621827</v>
       </c>
-      <c r="M36">
+      <c r="F48">
         <v>1622575</v>
       </c>
-      <c r="N36">
+      <c r="G48">
         <v>1623656</v>
       </c>
-      <c r="O36">
+      <c r="H48">
         <v>1615397</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>441529</v>
+      </c>
+      <c r="E49">
+        <v>438336</v>
+      </c>
+      <c r="F49">
+        <v>440769</v>
+      </c>
+      <c r="G49">
+        <v>441688</v>
+      </c>
+      <c r="H49">
+        <v>439772</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>1767092</v>
+      </c>
+      <c r="E50">
+        <v>1768499</v>
+      </c>
+      <c r="F50">
+        <v>1760107</v>
+      </c>
+      <c r="G50">
+        <v>1762926</v>
+      </c>
+      <c r="H50">
+        <v>1759054</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52">
+        <v>1545043</v>
+      </c>
+      <c r="E52">
+        <v>1539963</v>
+      </c>
+      <c r="F52">
+        <v>1542107</v>
+      </c>
+      <c r="G52">
+        <v>1555455</v>
+      </c>
+      <c r="H52">
+        <v>1549895</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>2205729</v>
+      </c>
+      <c r="E53">
+        <v>2219628</v>
+      </c>
+      <c r="F53">
+        <v>2219855</v>
+      </c>
+      <c r="G53">
+        <v>2209528</v>
+      </c>
+      <c r="H53">
+        <v>2214837</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54">
+        <v>1612530</v>
+      </c>
+      <c r="E54">
+        <v>1621726</v>
+      </c>
+      <c r="F54">
+        <v>1618473</v>
+      </c>
+      <c r="G54">
+        <v>1620487</v>
+      </c>
+      <c r="H54">
+        <v>1620762</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>438422</v>
+      </c>
+      <c r="E55">
+        <v>439556</v>
+      </c>
+      <c r="F55">
+        <v>440640</v>
+      </c>
+      <c r="G55">
+        <v>440996</v>
+      </c>
+      <c r="H55">
+        <v>440913</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>1754557</v>
+      </c>
+      <c r="E56">
+        <v>1764297</v>
+      </c>
+      <c r="F56">
+        <v>1761706</v>
+      </c>
+      <c r="G56">
+        <v>1760685</v>
+      </c>
+      <c r="H56">
+        <v>1765900</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58">
+        <v>1544811</v>
+      </c>
+      <c r="E58">
+        <v>1545911</v>
+      </c>
+      <c r="F58">
+        <v>1557121</v>
+      </c>
+      <c r="G58">
+        <v>1554298</v>
+      </c>
+      <c r="H58">
+        <v>1554546</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>2208944</v>
+      </c>
+      <c r="E59">
+        <v>2202401</v>
+      </c>
+      <c r="F59">
+        <v>2205117</v>
+      </c>
+      <c r="G59">
+        <v>2227335</v>
+      </c>
+      <c r="H59">
+        <v>2205895</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60">
+        <v>1613975</v>
+      </c>
+      <c r="E60">
+        <v>1613966</v>
+      </c>
+      <c r="F60">
+        <v>1622120</v>
+      </c>
+      <c r="G60">
+        <v>1613111</v>
+      </c>
+      <c r="H60">
+        <v>1613473</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61">
+        <v>440199</v>
+      </c>
+      <c r="E61">
+        <v>441627</v>
+      </c>
+      <c r="F61">
+        <v>439332</v>
+      </c>
+      <c r="G61">
+        <v>441422</v>
+      </c>
+      <c r="H61">
+        <v>439328</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <v>1755539</v>
+      </c>
+      <c r="E62">
+        <v>1760969</v>
+      </c>
+      <c r="G62">
+        <v>1764796</v>
+      </c>
+      <c r="H62">
+        <v>1764320</v>
       </c>
     </row>
   </sheetData>
@@ -7357,19 +9805,19 @@
     <mergeCell ref="H15:I15"/>
   </mergeCells>
   <conditionalFormatting sqref="G17 K17">
-    <cfRule type="top10" dxfId="29" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="139" priority="1" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18 K18">
-    <cfRule type="top10" dxfId="28" priority="2" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="138" priority="2" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19 K19">
-    <cfRule type="top10" dxfId="27" priority="3" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="137" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20 K20">
-    <cfRule type="top10" dxfId="26" priority="4" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="136" priority="4" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G21 K21">
-    <cfRule type="top10" dxfId="25" priority="5" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="135" priority="5" bottom="1" rank="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>